<commit_message>
added sample place holders
</commit_message>
<xml_diff>
--- a/data_links.xlsx
+++ b/data_links.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rasmu\AppData\Roaming\MobaXterm\slash\RemoteFiles\526870_2_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rasmu\AppData\Roaming\MobaXterm\slash\RemoteFiles\526870_10_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E146E1E-628A-4DF1-B172-3EC0F43D4B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400E527B-6A92-42DD-842C-E7B833B83BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Sample</t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t>"/projects/MicroBench/data/ PAS01578.dorado0.7.3.bmdna_r10.4.1_e8.2_400bps@5.0.0_sup.dup.fastq.gz"</t>
+  </si>
+  <si>
+    <t>Anabaena variabilis PCC 7120 DSM 107007</t>
+  </si>
+  <si>
+    <t>Bacillus cereus NRS 248 ATCC 10987</t>
+  </si>
+  <si>
+    <t>ZymoGut</t>
+  </si>
+  <si>
+    <t>ZymoOral</t>
+  </si>
+  <si>
+    <t>ZymoFecal</t>
   </si>
 </sst>
 </file>
@@ -444,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,6 +605,31 @@
         <v>27</v>
       </c>
     </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1" xr:uid="{CEACE548-A38F-4EC6-9DAA-C772C0F5E7E2}"/>

</xml_diff>

<commit_message>
fixed some whitespace characters
</commit_message>
<xml_diff>
--- a/data_links.xlsx
+++ b/data_links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rasmu\AppData\Roaming\MobaXterm\slash\RemoteFiles\526870_10_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400E527B-6A92-42DD-842C-E7B833B83BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C530720B-A952-4F00-B4C6-A7452275592E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added fast and hac data
</commit_message>
<xml_diff>
--- a/data_links.xlsx
+++ b/data_links.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rasmu\AppData\Roaming\MobaXterm\slash\RemoteFiles\526870_10_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rasmu\AppData\Roaming\MobaXterm\slash\RemoteFiles\131710_4_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C530720B-A952-4F00-B4C6-A7452275592E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABA9150-0A8B-4C27-8147-635CA4B930C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Sample</t>
   </si>
@@ -66,9 +66,6 @@
     <t xml:space="preserve"> supdup</t>
   </si>
   <si>
-    <t xml:space="preserve"> allmods</t>
-  </si>
-  <si>
     <t>ZymoHMW</t>
   </si>
   <si>
@@ -124,6 +121,18 @@
   </si>
   <si>
     <t>ZymoFecal</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAS01578.dorado0.7.3.bmdna_r10.4.1_e8.2_400bps@5.0.0_hac.dup.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAS01578.dorado0.7.3.bmdna_r10.4.1_e8.2_400bps@5.0.0_hac.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>"/projects/MicroBench/data/.PAS01578.dorado0.7.3.bmdna_r10.4.1_e8.2_400bps@5.0.0_fast.sim.fastq.gz"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mods</t>
   </si>
 </sst>
 </file>
@@ -462,7 +471,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="M1" t="s">
         <v>11</v>
@@ -523,111 +532,120 @@
         <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3">
         <v>45146</v>
       </c>
       <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
       </c>
       <c r="G2" s="2">
         <v>45276</v>
       </c>
       <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="N2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3">
         <v>45146</v>
       </c>
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
       </c>
       <c r="G3" s="2">
         <v>45548</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
       </c>
       <c r="M3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
         <v>26</v>
-      </c>
-      <c r="N3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added methylation data for zymohmw
</commit_message>
<xml_diff>
--- a/data_links.xlsx
+++ b/data_links.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rasmu\AppData\Roaming\MobaXterm\slash\RemoteFiles\131710_4_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UR36RV\AppData\Roaming\MobaXterm\slash\RemoteFiles\264364_4_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ADB0693-D4CE-4A07-BA00-112585AF4F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F268EAB2-7582-4A11-A8BA-22A376CAC4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Sample</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>/projects/MicroBench/data/PAS01578.dorado0.7.3.bmdna_r10.4.1_e8.2_400bps@5.0.0_fast.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAS01578.dorado0.7.3.bmdna_r10.4.1_e8.2_400bps@5.0.0_sup.sim.mod4mC_5mC_6mA.bam</t>
   </si>
 </sst>
 </file>
@@ -471,7 +474,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,6 +625,9 @@
       <c r="N3" t="s">
         <v>34</v>
       </c>
+      <c r="O3" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -651,6 +657,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="M2" r:id="rId1" xr:uid="{CEACE548-A38F-4EC6-9DAA-C772C0F5E7E2}"/>
+    <hyperlink ref="O3" r:id="rId2" display="PAS01578.dorado0.7.3.bmdna_r10.4.1_e8.2_400bps@5.0.0_sup.sim.mod4mC_5mC_6mA.bam" xr:uid="{E3AB7246-D3A6-4762-ABA2-71620A63D23E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added placeholders for real metagenomes
</commit_message>
<xml_diff>
--- a/data_links.xlsx
+++ b/data_links.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UR36RV\AppData\Roaming\MobaXterm\slash\RemoteFiles\264364_4_5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rasmu\AppData\Roaming\MobaXterm\slash\RemoteFiles\1115130_2_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F268EAB2-7582-4A11-A8BA-22A376CAC4B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9EE2A4-3906-47AC-925A-57578F361C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="14400" windowHeight="8350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t>Sample</t>
   </si>
@@ -136,6 +136,18 @@
   </si>
   <si>
     <t>/projects/MicroBench/data/PAS01578.dorado0.7.3.bmdna_r10.4.1_e8.2_400bps@5.0.0_sup.sim.mod4mC_5mC_6mA.bam</t>
+  </si>
+  <si>
+    <t>LSK114</t>
+  </si>
+  <si>
+    <t>FLO-PRO114M</t>
+  </si>
+  <si>
+    <t>5 khz</t>
+  </si>
+  <si>
+    <t>PAW77640</t>
   </si>
 </sst>
 </file>
@@ -474,24 +486,24 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +550,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -582,7 +594,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -629,29 +641,44 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>29</v>
+      </c>
+      <c r="B8" s="2">
+        <v>45566</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added path to zymo oral data
</commit_message>
<xml_diff>
--- a/data_links.xlsx
+++ b/data_links.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UR36RV\AppData\Roaming\MobaXterm\slash\RemoteFiles\264146_4_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UR36RV\AppData\Roaming\MobaXterm\slash\RemoteFiles\1050752_9_8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA87A197-ED49-46F2-829C-4CD8B66034C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9422EEAD-C6FA-4332-95BE-2A01E9F6870C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>Sample</t>
   </si>
@@ -160,6 +160,18 @@
   </si>
   <si>
     <t>0.8.1</t>
+  </si>
+  <si>
+    <t>PAY12289</t>
+  </si>
+  <si>
+    <t>0.8.2</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAY12289_barcode12.dorado0.8.2.bm5.0.0.sup.mod4mC_5mC_6mA.bam</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAY12289_barcode13.dorado0.8.2.bm5.0.0.sup.mod4mC_5mC_6mA.bam</t>
   </si>
 </sst>
 </file>
@@ -498,7 +510,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,20 +669,74 @@
       <c r="A4" t="s">
         <v>25</v>
       </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
+      <c r="B6" s="2">
+        <v>45590</v>
+      </c>
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="2">
+        <v>45593</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
+      </c>
+      <c r="B7" s="2">
+        <v>45590</v>
+      </c>
+      <c r="D7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="2">
+        <v>45594</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" t="s">
+        <v>43</v>
+      </c>
+      <c r="O7" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated with mono cultures
</commit_message>
<xml_diff>
--- a/data_links.xlsx
+++ b/data_links.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UR36RV\AppData\Roaming\MobaXterm\slash\RemoteFiles\1050752_9_8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rasmu\AppData\Roaming\MobaXterm\slash\RemoteFiles\198250_4_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9422EEAD-C6FA-4332-95BE-2A01E9F6870C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCF607F-B20F-41C2-89C8-FF50BCF73A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="133">
   <si>
     <t>Sample</t>
   </si>
@@ -105,9 +116,6 @@
     <t>Anabaena variabilis PCC 7120 DSM 107007</t>
   </si>
   <si>
-    <t>Bacillus cereus NRS 248 ATCC 10987</t>
-  </si>
-  <si>
     <t>ZymoGut</t>
   </si>
   <si>
@@ -172,13 +180,268 @@
   </si>
   <si>
     <t>/projects/MicroBench/data/PAY12289_barcode13.dorado0.8.2.bm5.0.0.sup.mod4mC_5mC_6mA.bam</t>
+  </si>
+  <si>
+    <t>SQK-NBD114.24</t>
+  </si>
+  <si>
+    <t>SQK-RBK114.24</t>
+  </si>
+  <si>
+    <t>PAW78174</t>
+  </si>
+  <si>
+    <t>Thermanaerovibrio acidaminovorans Su883 DSM 6589</t>
+  </si>
+  <si>
+    <t>Sphaerotilus natans 6 DSM 6575</t>
+  </si>
+  <si>
+    <t>Methanocaldococcus jannaschii JAL-1 DSM 2661</t>
+  </si>
+  <si>
+    <t>Sagittula stellata E-37 DSM 11524</t>
+  </si>
+  <si>
+    <t>Burkholderia cenocepacia J2315 DSM 16553</t>
+  </si>
+  <si>
+    <t>Salmonella bongori 1224.72 DSM 13772</t>
+  </si>
+  <si>
+    <t>Zymomonas mobilis subsp. pomaceae Barker I DSM 22645</t>
+  </si>
+  <si>
+    <t>Pelobacter carbinolicus Bd1 DSM 2380</t>
+  </si>
+  <si>
+    <t>Sphaerobacter thermophilus S 6022 DSM 20745</t>
+  </si>
+  <si>
+    <t>Desulfobacca acetoxidans ASRB2 DSM 11109</t>
+  </si>
+  <si>
+    <t>pod5</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/pod5/PAW78174_barcode01/</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/pod5/PAW78174_barcode02/</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/pod5/PAW78174_barcode03/</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/pod5/PAW78174_barcode04/</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/pod5/PAW78174_barcode05/</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/pod5/PAW78174_barcode06/</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/pod5/PAW78174_barcode07/</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/pod5/PAW78174_barcode08/</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/pod5/PAW78174_barcode09/</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/pod5/PAW78174_barcode10/</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/pod5/PAW78174_barcode11/</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode01.dorado0.8.2.bm5.0.0.fast.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode02.dorado0.8.2.bm5.0.0.fast.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode03.dorado0.8.2.bm5.0.0.fast.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode04.dorado0.8.2.bm5.0.0.fast.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode05.dorado0.8.2.bm5.0.0.fast.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode06.dorado0.8.2.bm5.0.0.fast.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode07.dorado0.8.2.bm5.0.0.fast.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode08.dorado0.8.2.bm5.0.0.fast.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode09.dorado0.8.2.bm5.0.0.fast.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode10.dorado0.8.2.bm5.0.0.fast.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode01.dorado0.8.2.bm5.0.0.hac.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode01.dorado0.8.2.bm5.0.0.sup.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode02.dorado0.8.2.bm5.0.0.hac.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode02.dorado0.8.2.bm5.0.0.sup.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode03.dorado0.8.2.bm5.0.0.hac.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode03.dorado0.8.2.bm5.0.0.sup.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode04.dorado0.8.2.bm5.0.0.hac.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode04.dorado0.8.2.bm5.0.0.sup.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode05.dorado0.8.2.bm5.0.0.hac.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode05.dorado0.8.2.bm5.0.0.sup.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode06.dorado0.8.2.bm5.0.0.hac.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode06.dorado0.8.2.bm5.0.0.sup.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode07.dorado0.8.2.bm5.0.0.hac.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode07.dorado0.8.2.bm5.0.0.sup.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode08.dorado0.8.2.bm5.0.0.hac.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode08.dorado0.8.2.bm5.0.0.sup.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode09.dorado0.8.2.bm5.0.0.hac.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode09.dorado0.8.2.bm5.0.0.sup.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode10.dorado0.8.2.bm5.0.0.hac.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode10.dorado0.8.2.bm5.0.0.sup.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode1.dorado0.8.2.bm5.0.0.fast.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode1.dorado0.8.2.bm5.0.0.hac.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW78174_barcode1.dorado0.8.2.bm5.0.0.sup.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/pod5/PAS01578/</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/pod5/PAY12289_barcode13/</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/pod5/PAY12289_barcode12/</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/pod5/PAW77640/</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/.PAW77640.dorado0.8.2.bm5.0.0.fast.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/.PAW77640.dorado0.8.2.bm5.0.0.hac.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/.PAW77640.dorado0.8.2.bm5.0.0.sup.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>SampleType</t>
+  </si>
+  <si>
+    <t>mock</t>
+  </si>
+  <si>
+    <t>monoculture</t>
+  </si>
+  <si>
+    <t>metagenome</t>
+  </si>
+  <si>
+    <t>SampleInfo</t>
+  </si>
+  <si>
+    <t>https://zymoresearch.eu/products/zymobiomics-gut-microbiome-standard</t>
+  </si>
+  <si>
+    <t>https://zymoresearch.eu/products/zymobiomics-hmw-dna-standard</t>
+  </si>
+  <si>
+    <t>https://zymoresearch.eu/products/zymobiomics-oral-microbiome-standard</t>
+  </si>
+  <si>
+    <t>https://zymoresearch.eu/collections/zymobiomics-microbial-community-standards/products/zymobiomics-fecal-reference-with-trumatrix-technology</t>
+  </si>
+  <si>
+    <t>https://www.dsmz.de/collection/catalogue/details/culture/DSM-107007</t>
+  </si>
+  <si>
+    <t>https://www.dsmz.de/collection/catalogue/details/culture/DSM-6589</t>
+  </si>
+  <si>
+    <t>https://www.dsmz.de/collection/catalogue/details/culture/DSM-6575</t>
+  </si>
+  <si>
+    <t>https://www.dsmz.de/collection/catalogue/details/culture/DSM-2661</t>
+  </si>
+  <si>
+    <t>https://www.dsmz.de/collection/catalogue/details/culture/DSM-11524</t>
+  </si>
+  <si>
+    <t>https://www.dsmz.de/collection/catalogue/details/culture/DSM-16553</t>
+  </si>
+  <si>
+    <t>https://www.dsmz.de/collection/catalogue/details/culture/DSM-13772</t>
+  </si>
+  <si>
+    <t>https://www.dsmz.de/collection/catalogue/details/culture/DSM-22645</t>
+  </si>
+  <si>
+    <t>https://www.dsmz.de/collection/catalogue/details/culture/DSM-2380</t>
+  </si>
+  <si>
+    <t>https://www.dsmz.de/collection/catalogue/details/culture/DSM-20745</t>
+  </si>
+  <si>
+    <t>https://www.dsmz.de/collection/catalogue/details/culture/DSM-11109</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +461,12 @@
       <sz val="9"/>
       <color rgb="FF1F1F1F"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -507,304 +776,978 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="38.453125" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="3">
         <v>45146</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="2">
+      <c r="I2" s="2">
         <v>45276</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
       </c>
       <c r="L2" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="3">
         <v>45146</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="2">
+      <c r="I3" s="2">
         <v>45548</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>21</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="R3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45590</v>
+      </c>
+      <c r="E4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="2">
+        <v>45593</v>
+      </c>
+      <c r="J4" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="2">
+        <v>45590</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="2">
+        <v>45594</v>
+      </c>
+      <c r="J5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>46</v>
+      </c>
+      <c r="R5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="2">
+        <v>45566</v>
+      </c>
+      <c r="E6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="2">
-        <v>45590</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="H6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6" s="2">
-        <v>45593</v>
-      </c>
-      <c r="H6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" t="s">
-        <v>43</v>
+      <c r="I6" s="2">
+        <v>45570</v>
+      </c>
+      <c r="J6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" t="s">
+        <v>20</v>
       </c>
       <c r="O6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="P6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>40</v>
+      </c>
+      <c r="R6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="2">
-        <v>45590</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D7" s="2">
+        <v>45566</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" t="s">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
+      <c r="I7" s="2">
+        <v>45604</v>
+      </c>
+      <c r="J7" t="s">
         <v>45</v>
       </c>
-      <c r="F7" t="s">
+      <c r="K7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" t="s">
+        <v>110</v>
+      </c>
+      <c r="M7" t="s">
+        <v>111</v>
+      </c>
+      <c r="O7" t="s">
+        <v>112</v>
+      </c>
+      <c r="R7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="2">
+        <v>45566</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="2">
-        <v>45594</v>
-      </c>
-      <c r="H7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="2">
+        <v>45572</v>
+      </c>
+      <c r="J8" t="s">
         <v>43</v>
       </c>
-      <c r="O7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="2">
-        <v>45566</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="K8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" t="s">
         <v>37</v>
       </c>
-      <c r="D8" t="s">
+      <c r="G9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" t="s">
         <v>38</v>
       </c>
-      <c r="E8" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="2">
-        <v>45570</v>
-      </c>
-      <c r="H8" t="s">
+      <c r="I9" s="2">
+        <v>45601</v>
+      </c>
+      <c r="J9" t="s">
+        <v>45</v>
+      </c>
+      <c r="K9" t="s">
         <v>42</v>
       </c>
-      <c r="I8" t="s">
-        <v>43</v>
-      </c>
-      <c r="O8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="2">
-        <v>45566</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="L9" t="s">
+        <v>73</v>
+      </c>
+      <c r="M9" t="s">
+        <v>83</v>
+      </c>
+      <c r="O9" t="s">
+        <v>84</v>
+      </c>
+      <c r="R9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="G10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="2">
-        <v>45572</v>
-      </c>
-      <c r="H9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I9" t="s">
-        <v>43</v>
-      </c>
+      <c r="I10" s="2">
+        <v>45603</v>
+      </c>
+      <c r="J10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" t="s">
+        <v>74</v>
+      </c>
+      <c r="M10" t="s">
+        <v>85</v>
+      </c>
+      <c r="O10" t="s">
+        <v>86</v>
+      </c>
+      <c r="R10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11" s="2">
+        <v>45603</v>
+      </c>
+      <c r="J11" t="s">
+        <v>45</v>
+      </c>
+      <c r="K11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" t="s">
+        <v>75</v>
+      </c>
+      <c r="M11" t="s">
+        <v>87</v>
+      </c>
+      <c r="O11" t="s">
+        <v>88</v>
+      </c>
+      <c r="R11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" t="s">
+        <v>50</v>
+      </c>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="2">
+        <v>45603</v>
+      </c>
+      <c r="J12" t="s">
+        <v>45</v>
+      </c>
+      <c r="K12" t="s">
+        <v>42</v>
+      </c>
+      <c r="L12" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" t="s">
+        <v>89</v>
+      </c>
+      <c r="O12" t="s">
+        <v>90</v>
+      </c>
+      <c r="R12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13" s="2">
+        <v>45603</v>
+      </c>
+      <c r="J13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" t="s">
+        <v>77</v>
+      </c>
+      <c r="M13" t="s">
+        <v>91</v>
+      </c>
+      <c r="O13" t="s">
+        <v>92</v>
+      </c>
+      <c r="R13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="2">
+        <v>45603</v>
+      </c>
+      <c r="J14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K14" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" t="s">
+        <v>78</v>
+      </c>
+      <c r="M14" t="s">
+        <v>93</v>
+      </c>
+      <c r="O14" t="s">
+        <v>94</v>
+      </c>
+      <c r="R14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15" s="2">
+        <v>45603</v>
+      </c>
+      <c r="J15" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" t="s">
+        <v>42</v>
+      </c>
+      <c r="L15" t="s">
+        <v>79</v>
+      </c>
+      <c r="M15" t="s">
+        <v>95</v>
+      </c>
+      <c r="O15" t="s">
+        <v>96</v>
+      </c>
+      <c r="R15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16" s="2">
+        <v>45603</v>
+      </c>
+      <c r="J16" t="s">
+        <v>45</v>
+      </c>
+      <c r="K16" t="s">
+        <v>42</v>
+      </c>
+      <c r="L16" t="s">
+        <v>80</v>
+      </c>
+      <c r="M16" t="s">
+        <v>97</v>
+      </c>
+      <c r="O16" t="s">
+        <v>98</v>
+      </c>
+      <c r="R16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" t="s">
+        <v>50</v>
+      </c>
+      <c r="H17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17" s="2">
+        <v>45603</v>
+      </c>
+      <c r="J17" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" t="s">
+        <v>42</v>
+      </c>
+      <c r="L17" t="s">
+        <v>81</v>
+      </c>
+      <c r="M17" t="s">
+        <v>99</v>
+      </c>
+      <c r="O17" t="s">
+        <v>100</v>
+      </c>
+      <c r="R17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>115</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E18" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H18" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="2">
+        <v>45603</v>
+      </c>
+      <c r="J18" t="s">
+        <v>45</v>
+      </c>
+      <c r="K18" t="s">
+        <v>42</v>
+      </c>
+      <c r="L18" t="s">
+        <v>82</v>
+      </c>
+      <c r="M18" t="s">
+        <v>101</v>
+      </c>
+      <c r="O18" t="s">
+        <v>102</v>
+      </c>
+      <c r="R18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="2">
+        <v>45603</v>
+      </c>
+      <c r="J19" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" t="s">
+        <v>42</v>
+      </c>
+      <c r="L19" t="s">
+        <v>103</v>
+      </c>
+      <c r="M19" t="s">
+        <v>104</v>
+      </c>
+      <c r="O19" t="s">
+        <v>105</v>
+      </c>
+      <c r="R19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D20" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="M2" r:id="rId1" xr:uid="{CEACE548-A38F-4EC6-9DAA-C772C0F5E7E2}"/>
-    <hyperlink ref="O3" r:id="rId2" display="PAS01578.dorado0.7.3.bmdna_r10.4.1_e8.2_400bps@5.0.0_sup.sim.mod4mC_5mC_6mA.bam" xr:uid="{E3AB7246-D3A6-4762-ABA2-71620A63D23E}"/>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{CEACE548-A38F-4EC6-9DAA-C772C0F5E7E2}"/>
+    <hyperlink ref="Q3" r:id="rId2" display="PAS01578.dorado0.7.3.bmdna_r10.4.1_e8.2_400bps@5.0.0_sup.sim.mod4mC_5mC_6mA.bam" xr:uid="{E3AB7246-D3A6-4762-ABA2-71620A63D23E}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{0B0682C5-AF89-4A3B-88B3-B7BB30CF94C5}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{95A85873-7B30-41C5-B9EC-B9195C3B8A60}"/>
+    <hyperlink ref="C4" r:id="rId5" xr:uid="{5A6BC38D-CD7A-436D-8357-B390C66C9FE6}"/>
+    <hyperlink ref="C5" r:id="rId6" xr:uid="{AB054604-E404-4365-8D34-43BE4C2945D8}"/>
+    <hyperlink ref="C6" r:id="rId7" xr:uid="{1ACA7579-C420-409C-87A6-14C552E3EF91}"/>
+    <hyperlink ref="C7" r:id="rId8" xr:uid="{E5953102-439B-443A-AAA8-0922C96D5322}"/>
+    <hyperlink ref="C8" r:id="rId9" xr:uid="{6921DD9E-2E31-4F93-898F-4ADF1C2B5BF4}"/>
+    <hyperlink ref="C9" r:id="rId10" xr:uid="{8F0A319C-C30F-403C-9FBD-DA7A6D9E7F72}"/>
+    <hyperlink ref="C10" r:id="rId11" xr:uid="{522041E2-0A70-4401-A33D-7105607D3C2C}"/>
+    <hyperlink ref="C11" r:id="rId12" xr:uid="{5377E8DC-7C9C-486C-93BB-9CE37B5265A1}"/>
+    <hyperlink ref="C12" r:id="rId13" xr:uid="{7EDB0F78-6FD9-426D-9C0A-3B2318EF9D17}"/>
+    <hyperlink ref="C13" r:id="rId14" xr:uid="{25D5AD65-19E9-464F-82AB-A1DFE024AE3C}"/>
+    <hyperlink ref="C14" r:id="rId15" xr:uid="{062A9CDF-1CCF-4BDE-9557-A88B58F21D39}"/>
+    <hyperlink ref="C15" r:id="rId16" xr:uid="{6C21CCD9-BCB2-4B98-9472-4802BCB12B35}"/>
+    <hyperlink ref="C16" r:id="rId17" xr:uid="{28B3D1C4-C19D-496E-BCAD-A81E4FDF9AE3}"/>
+    <hyperlink ref="C17" r:id="rId18" xr:uid="{9F3B402C-4D42-43F6-81A7-F997095086B2}"/>
+    <hyperlink ref="C18" r:id="rId19" xr:uid="{6E76EBCA-B825-4DB9-9FA2-1E291D576C07}"/>
+    <hyperlink ref="C19" r:id="rId20" xr:uid="{79193C2B-03CA-4734-B402-D724B41E278D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added modification data for zymo fecal
</commit_message>
<xml_diff>
--- a/data_links.xlsx
+++ b/data_links.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rasmu\AppData\Roaming\MobaXterm\slash\RemoteFiles\198250_4_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UR36RV\AppData\Roaming\MobaXterm\slash\mx86_64b\RemoteFiles\460164_4_0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BCF607F-B20F-41C2-89C8-FF50BCF73A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EAF10B0-C359-4E28-AA43-D130562C3E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="139">
   <si>
     <t>Sample</t>
   </si>
@@ -98,9 +98,6 @@
     <t>ftp://ftp.sra.ebi.ac.uk/vol1/run/ERR119/ERR11901474/PAS01578.dna_r10.4.1_e8.2_400bps_sup@v4.2.0.fastq.gz</t>
   </si>
   <si>
-    <t>NA</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0.7.3</t>
   </si>
   <si>
@@ -435,6 +432,27 @@
   </si>
   <si>
     <t>https://www.dsmz.de/collection/catalogue/details/culture/DSM-11109</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAY12289_barcode13.dorado0.8.2.bm5.0.0.fast.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAY12289_barcode13.dorado0.8.2.bm5.0.0.hac.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAW77640.dorado0.8.2.bm5.0.0.sup.sim.mod4mC_5mC_6mA.bam</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAY12289_barcode13.dorado0.8.2.bm5.0.0.sup.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAY12289_barcode12.dorado0.8.2.bm5.0.0.fast.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAY12289_barcode12.dorado0.8.2.bm5.0.0.hac.sim.fastq.gz</t>
+  </si>
+  <si>
+    <t>/projects/MicroBench/data/PAY12289_barcode12.dorado0.8.2.bm5.0.0.sup.sim.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -779,33 +797,35 @@
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="38.453125" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -838,7 +858,7 @@
         <v>10</v>
       </c>
       <c r="N1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O1" t="s">
         <v>11</v>
@@ -847,556 +867,535 @@
         <v>12</v>
       </c>
       <c r="Q1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D2" s="3">
-        <v>45146</v>
+        <v>120</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45566</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I2" s="2">
-        <v>45276</v>
+        <v>45570</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" t="s">
-        <v>19</v>
+        <v>41</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>39</v>
       </c>
       <c r="R2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D3" s="3">
-        <v>45146</v>
+        <v>120</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45566</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="I3" s="2">
-        <v>45548</v>
+        <v>45572</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="K3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="2">
+        <v>45566</v>
+      </c>
+      <c r="E4" t="s">
         <v>35</v>
       </c>
-      <c r="R3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="2">
-        <v>45590</v>
-      </c>
-      <c r="E4" t="s">
-        <v>48</v>
-      </c>
       <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" t="s">
         <v>37</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" s="2">
+        <v>45604</v>
+      </c>
+      <c r="J4" t="s">
         <v>44</v>
       </c>
-      <c r="H4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" s="2">
-        <v>45593</v>
-      </c>
-      <c r="J4" t="s">
-        <v>45</v>
-      </c>
       <c r="K4" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
+        <v>109</v>
+      </c>
+      <c r="M4" t="s">
+        <v>110</v>
+      </c>
+      <c r="O4" t="s">
+        <v>111</v>
       </c>
       <c r="Q4" t="s">
-        <v>47</v>
+        <v>134</v>
       </c>
       <c r="R4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D5" s="2">
         <v>45590</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
         <v>37</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" s="2">
+        <v>45593</v>
+      </c>
+      <c r="J5" t="s">
         <v>44</v>
       </c>
-      <c r="H5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="2">
-        <v>45594</v>
-      </c>
-      <c r="J5" t="s">
-        <v>45</v>
-      </c>
       <c r="K5" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="L5" t="s">
+        <v>132</v>
+      </c>
+      <c r="M5" t="s">
+        <v>133</v>
+      </c>
+      <c r="O5" t="s">
+        <v>135</v>
       </c>
       <c r="Q5" t="s">
         <v>46</v>
       </c>
       <c r="R5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="3">
+        <v>45146</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="2">
+        <v>45276</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="3">
+        <v>45146</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="2">
+        <v>45548</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" t="s">
         <v>28</v>
       </c>
-      <c r="B6" t="s">
-        <v>116</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="O7" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>113</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="2">
+        <v>45590</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="2">
+        <v>45594</v>
+      </c>
+      <c r="J8" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" t="s">
+        <v>41</v>
+      </c>
+      <c r="L8" t="s">
+        <v>136</v>
+      </c>
+      <c r="M8" t="s">
+        <v>137</v>
+      </c>
+      <c r="O8" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>45</v>
+      </c>
+      <c r="R8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="D6" s="2">
-        <v>45566</v>
-      </c>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I6" s="2">
-        <v>45570</v>
-      </c>
-      <c r="J6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" t="s">
-        <v>20</v>
-      </c>
-      <c r="M6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" t="s">
-        <v>20</v>
-      </c>
-      <c r="O6" t="s">
-        <v>20</v>
-      </c>
-      <c r="P6" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>40</v>
-      </c>
-      <c r="R6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D7" s="2">
-        <v>45566</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="2">
-        <v>45604</v>
-      </c>
-      <c r="J7" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" t="s">
-        <v>42</v>
-      </c>
-      <c r="L7" t="s">
-        <v>110</v>
-      </c>
-      <c r="M7" t="s">
-        <v>111</v>
-      </c>
-      <c r="O7" t="s">
-        <v>112</v>
-      </c>
-      <c r="R7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D8" s="2">
-        <v>45566</v>
-      </c>
-      <c r="E8" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="2">
-        <v>45572</v>
-      </c>
-      <c r="J8" t="s">
-        <v>43</v>
-      </c>
-      <c r="K8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" t="s">
-        <v>20</v>
-      </c>
-      <c r="O8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P8" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>20</v>
-      </c>
-      <c r="R8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="D9" s="2">
         <v>45597</v>
       </c>
       <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
         <v>49</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>37</v>
-      </c>
-      <c r="G9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" t="s">
-        <v>38</v>
       </c>
       <c r="I9" s="2">
         <v>45601</v>
       </c>
       <c r="J9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M9" t="s">
+        <v>82</v>
+      </c>
+      <c r="O9" t="s">
         <v>83</v>
       </c>
-      <c r="O9" t="s">
-        <v>84</v>
-      </c>
       <c r="R9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D10" s="2">
         <v>45597</v>
       </c>
       <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" t="s">
         <v>49</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>37</v>
-      </c>
-      <c r="G10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" t="s">
-        <v>38</v>
       </c>
       <c r="I10" s="2">
         <v>45603</v>
       </c>
       <c r="J10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L10" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="M10" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="O10" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="R10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D11" s="2">
         <v>45597</v>
       </c>
       <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
         <v>49</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>37</v>
-      </c>
-      <c r="G11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" t="s">
-        <v>38</v>
       </c>
       <c r="I11" s="2">
         <v>45603</v>
       </c>
       <c r="J11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="M11" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="O11" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="R11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D12" s="2">
         <v>45597</v>
       </c>
       <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12" t="s">
         <v>49</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>37</v>
-      </c>
-      <c r="G12" t="s">
-        <v>50</v>
-      </c>
-      <c r="H12" t="s">
-        <v>38</v>
       </c>
       <c r="I12" s="2">
         <v>45603</v>
       </c>
       <c r="J12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M12" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="O12" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="R12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>126</v>
@@ -1405,92 +1404,92 @@
         <v>45597</v>
       </c>
       <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>36</v>
+      </c>
+      <c r="G13" t="s">
         <v>49</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>37</v>
-      </c>
-      <c r="G13" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" t="s">
-        <v>38</v>
       </c>
       <c r="I13" s="2">
         <v>45603</v>
       </c>
       <c r="J13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L13" t="s">
         <v>77</v>
       </c>
       <c r="M13" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="O13" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="R13" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D14" s="2">
         <v>45597</v>
       </c>
       <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" t="s">
         <v>49</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
         <v>37</v>
-      </c>
-      <c r="G14" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" t="s">
-        <v>38</v>
       </c>
       <c r="I14" s="2">
         <v>45603</v>
       </c>
       <c r="J14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="M14" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="O14" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="R14" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>128</v>
@@ -1499,45 +1498,45 @@
         <v>45597</v>
       </c>
       <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" t="s">
         <v>49</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>37</v>
-      </c>
-      <c r="G15" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15" t="s">
-        <v>38</v>
       </c>
       <c r="I15" s="2">
         <v>45603</v>
       </c>
       <c r="J15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L15" t="s">
         <v>79</v>
       </c>
       <c r="M15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="R15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>57</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>129</v>
@@ -1546,208 +1545,211 @@
         <v>45597</v>
       </c>
       <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" t="s">
         <v>49</v>
       </c>
-      <c r="F16" t="s">
+      <c r="H16" t="s">
         <v>37</v>
-      </c>
-      <c r="G16" t="s">
-        <v>50</v>
-      </c>
-      <c r="H16" t="s">
-        <v>38</v>
       </c>
       <c r="I16" s="2">
         <v>45603</v>
       </c>
       <c r="J16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L16" t="s">
         <v>80</v>
       </c>
       <c r="M16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="R16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D17" s="2">
         <v>45597</v>
       </c>
       <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" t="s">
         <v>49</v>
       </c>
-      <c r="F17" t="s">
+      <c r="H17" t="s">
         <v>37</v>
-      </c>
-      <c r="G17" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" t="s">
-        <v>38</v>
       </c>
       <c r="I17" s="2">
         <v>45603</v>
       </c>
       <c r="J17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L17" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="M17" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="O17" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="R17" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="D18" s="2">
         <v>45597</v>
       </c>
       <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" t="s">
         <v>49</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>37</v>
-      </c>
-      <c r="G18" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" t="s">
-        <v>38</v>
       </c>
       <c r="I18" s="2">
         <v>45603</v>
       </c>
       <c r="J18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L18" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="M18" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="O18" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="R18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="D19" s="2">
         <v>45597</v>
       </c>
       <c r="E19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G19" t="s">
         <v>49</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
         <v>37</v>
-      </c>
-      <c r="G19" t="s">
-        <v>50</v>
-      </c>
-      <c r="H19" t="s">
-        <v>38</v>
       </c>
       <c r="I19" s="2">
         <v>45603</v>
       </c>
       <c r="J19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L19" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="M19" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="O19" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="R19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D20" s="2"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R19">
+    <sortCondition ref="B2:B19"/>
+    <sortCondition ref="C2:C19"/>
+    <sortCondition ref="J2:J19"/>
+  </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" xr:uid="{CEACE548-A38F-4EC6-9DAA-C772C0F5E7E2}"/>
-    <hyperlink ref="Q3" r:id="rId2" display="PAS01578.dorado0.7.3.bmdna_r10.4.1_e8.2_400bps@5.0.0_sup.sim.mod4mC_5mC_6mA.bam" xr:uid="{E3AB7246-D3A6-4762-ABA2-71620A63D23E}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{0B0682C5-AF89-4A3B-88B3-B7BB30CF94C5}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{95A85873-7B30-41C5-B9EC-B9195C3B8A60}"/>
-    <hyperlink ref="C4" r:id="rId5" xr:uid="{5A6BC38D-CD7A-436D-8357-B390C66C9FE6}"/>
-    <hyperlink ref="C5" r:id="rId6" xr:uid="{AB054604-E404-4365-8D34-43BE4C2945D8}"/>
-    <hyperlink ref="C6" r:id="rId7" xr:uid="{1ACA7579-C420-409C-87A6-14C552E3EF91}"/>
-    <hyperlink ref="C7" r:id="rId8" xr:uid="{E5953102-439B-443A-AAA8-0922C96D5322}"/>
-    <hyperlink ref="C8" r:id="rId9" xr:uid="{6921DD9E-2E31-4F93-898F-4ADF1C2B5BF4}"/>
-    <hyperlink ref="C9" r:id="rId10" xr:uid="{8F0A319C-C30F-403C-9FBD-DA7A6D9E7F72}"/>
-    <hyperlink ref="C10" r:id="rId11" xr:uid="{522041E2-0A70-4401-A33D-7105607D3C2C}"/>
-    <hyperlink ref="C11" r:id="rId12" xr:uid="{5377E8DC-7C9C-486C-93BB-9CE37B5265A1}"/>
-    <hyperlink ref="C12" r:id="rId13" xr:uid="{7EDB0F78-6FD9-426D-9C0A-3B2318EF9D17}"/>
-    <hyperlink ref="C13" r:id="rId14" xr:uid="{25D5AD65-19E9-464F-82AB-A1DFE024AE3C}"/>
-    <hyperlink ref="C14" r:id="rId15" xr:uid="{062A9CDF-1CCF-4BDE-9557-A88B58F21D39}"/>
-    <hyperlink ref="C15" r:id="rId16" xr:uid="{6C21CCD9-BCB2-4B98-9472-4802BCB12B35}"/>
-    <hyperlink ref="C16" r:id="rId17" xr:uid="{28B3D1C4-C19D-496E-BCAD-A81E4FDF9AE3}"/>
-    <hyperlink ref="C17" r:id="rId18" xr:uid="{9F3B402C-4D42-43F6-81A7-F997095086B2}"/>
-    <hyperlink ref="C18" r:id="rId19" xr:uid="{6E76EBCA-B825-4DB9-9FA2-1E291D576C07}"/>
-    <hyperlink ref="C19" r:id="rId20" xr:uid="{79193C2B-03CA-4734-B402-D724B41E278D}"/>
+    <hyperlink ref="C6" r:id="rId1" xr:uid="{0B0682C5-AF89-4A3B-88B3-B7BB30CF94C5}"/>
+    <hyperlink ref="C7" r:id="rId2" xr:uid="{95A85873-7B30-41C5-B9EC-B9195C3B8A60}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{5A6BC38D-CD7A-436D-8357-B390C66C9FE6}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{AB054604-E404-4365-8D34-43BE4C2945D8}"/>
+    <hyperlink ref="C2" r:id="rId5" xr:uid="{1ACA7579-C420-409C-87A6-14C552E3EF91}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{E5953102-439B-443A-AAA8-0922C96D5322}"/>
+    <hyperlink ref="C3" r:id="rId7" xr:uid="{6921DD9E-2E31-4F93-898F-4ADF1C2B5BF4}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{8F0A319C-C30F-403C-9FBD-DA7A6D9E7F72}"/>
+    <hyperlink ref="C19" r:id="rId9" xr:uid="{522041E2-0A70-4401-A33D-7105607D3C2C}"/>
+    <hyperlink ref="C18" r:id="rId10" xr:uid="{5377E8DC-7C9C-486C-93BB-9CE37B5265A1}"/>
+    <hyperlink ref="C17" r:id="rId11" xr:uid="{7EDB0F78-6FD9-426D-9C0A-3B2318EF9D17}"/>
+    <hyperlink ref="C11" r:id="rId12" xr:uid="{25D5AD65-19E9-464F-82AB-A1DFE024AE3C}"/>
+    <hyperlink ref="C13" r:id="rId13" xr:uid="{062A9CDF-1CCF-4BDE-9557-A88B58F21D39}"/>
+    <hyperlink ref="C12" r:id="rId14" xr:uid="{6C21CCD9-BCB2-4B98-9472-4802BCB12B35}"/>
+    <hyperlink ref="C15" r:id="rId15" xr:uid="{28B3D1C4-C19D-496E-BCAD-A81E4FDF9AE3}"/>
+    <hyperlink ref="C16" r:id="rId16" xr:uid="{9F3B402C-4D42-43F6-81A7-F997095086B2}"/>
+    <hyperlink ref="C14" r:id="rId17" xr:uid="{6E76EBCA-B825-4DB9-9FA2-1E291D576C07}"/>
+    <hyperlink ref="C10" r:id="rId18" xr:uid="{79193C2B-03CA-4734-B402-D724B41E278D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId21"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added pod5 to ENA
</commit_message>
<xml_diff>
--- a/data_links.xlsx
+++ b/data_links.xlsx
@@ -516,7 +516,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAW77640/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789831/PAW77640.tar.gz</t>
         </is>
       </c>
     </row>
@@ -574,7 +574,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAW77640/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789831/PAW77640.tar.gz</t>
         </is>
       </c>
     </row>
@@ -652,7 +652,7 @@
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAW77640/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789831/PAW77640.tar.gz</t>
         </is>
       </c>
     </row>
@@ -730,7 +730,7 @@
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAY12289_barcode13/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789832/PAY12289_barcode13.tar.gz</t>
         </is>
       </c>
     </row>
@@ -798,7 +798,7 @@
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAS01578/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789833/PAS01578.tar.gz</t>
         </is>
       </c>
     </row>
@@ -886,7 +886,7 @@
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAS01578/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789833/PAS01578.tar.gz</t>
         </is>
       </c>
     </row>
@@ -964,7 +964,7 @@
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAY12289_barcode12/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789834/PAY12289_barcode12.tar.gz</t>
         </is>
       </c>
     </row>
@@ -1042,7 +1042,7 @@
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAW78174_barcode01/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789835/PAW78174_barcode01.tar.gz</t>
         </is>
       </c>
     </row>
@@ -1120,7 +1120,7 @@
       </c>
       <c r="R10" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAW78174_barcode11/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789836/PAW78174_barcode11.tar.gz</t>
         </is>
       </c>
     </row>
@@ -1198,7 +1198,7 @@
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAW78174_barcode05/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789837/PAW78174_barcode05.tar.gz</t>
         </is>
       </c>
     </row>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAW78174_barcode07/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789838/PAW78174_barcode07.tar.gz</t>
         </is>
       </c>
     </row>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAW78174_barcode06/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789839/PAW78174_barcode06.tar.gz</t>
         </is>
       </c>
     </row>
@@ -1432,7 +1432,7 @@
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAW78174_barcode10/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789840/PAW78174_barcode10.tar.gz</t>
         </is>
       </c>
     </row>
@@ -1510,7 +1510,7 @@
       </c>
       <c r="R15" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAW78174_barcode08/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789841/PAW78174_barcode08.tar.gz</t>
         </is>
       </c>
     </row>
@@ -1666,7 +1666,7 @@
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAW78174_barcode04/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789842/PAW78174_barcode04.tar.gz</t>
         </is>
       </c>
     </row>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAW78174_barcode03/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789843/PAW78174_barcode03.tar.gz</t>
         </is>
       </c>
     </row>
@@ -1822,7 +1822,7 @@
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>/projects/MicroBench/data/pod5/PAW78174_barcode02/</t>
+          <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789844/PAW78174_barcode02.tar.gz</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added 5.2.0 model data
</commit_message>
<xml_diff>
--- a/data_links.xlsx
+++ b/data_links.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UR36RV\AppData\Roaming\MobaXterm\slash\RemoteFiles\198514_4_0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UR36RV\AppData\Roaming\MobaXterm\slash\mx86_64b\RemoteFiles\131872_4_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470A980C-7F75-4E1F-AF1B-9C19F1B95A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC45C3E8-461C-4A30-AE67-1E8BF6F280D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="138">
   <si>
     <t>Sample</t>
   </si>
@@ -395,6 +395,45 @@
   </si>
   <si>
     <t>ftp.sra.ebi.ac.uk/vol1/run/ERR147/ERR14789844/PAW78174_barcode02.tar.gz</t>
+  </si>
+  <si>
+    <t>5.2.0</t>
+  </si>
+  <si>
+    <t>1.0.0</t>
+  </si>
+  <si>
+    <t>/projects/MA/RHK/MicroBench/data/PAS01578.dorado1.0.0.bm5.2.0_sup.sim.mod4mC_5mC_6mA.bam</t>
+  </si>
+  <si>
+    <t>/projects/MA/RHK/MicroBench/data/PAY12289_barcode12.dorado1.0.0.bm5.2.0_sup.sim.mod4mC_5mC_6mA.bam</t>
+  </si>
+  <si>
+    <t>/projects/MA/RHK/MicroBench/data/PAY12289_barcode13.dorado1.0.0.bm5.2.0_sup.sim.mod4mC_5mC_6mA.bam</t>
+  </si>
+  <si>
+    <t>MFD00392</t>
+  </si>
+  <si>
+    <t>MFD06742</t>
+  </si>
+  <si>
+    <t>https://github.com/cmc-aau/mfd_wiki/wiki/Metadata#minimal-metadata</t>
+  </si>
+  <si>
+    <t>PAQ96168</t>
+  </si>
+  <si>
+    <t>/projects/MA/RHK/MicroBench/data/MFD00392.dorado1.0.0.bm5.2.0_sup.sim.mod4mC_5mC_6mA.bam</t>
+  </si>
+  <si>
+    <t>PAQ67232</t>
+  </si>
+  <si>
+    <t>/projects/MA/RHK/MicroBench/data/MFD06742.dorado1.0.0.bm5.2.0_sup.sim.mod4mC_5mC_6mA.bam</t>
+  </si>
+  <si>
+    <t>/projects/MA/RHK/MicroBench/data/PAS01578.dorado1.0.0.bm5.2.0_fast.sim.bam</t>
   </si>
 </sst>
 </file>
@@ -404,7 +443,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss\ \U\T\C"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +455,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -441,12 +486,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,18 +797,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="139" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="129.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1196,7 +1245,7 @@
       <c r="Q9" t="s">
         <v>74</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R9" s="3" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1550,7 +1599,514 @@
         <v>124</v>
       </c>
     </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="2">
+        <v>45146</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="2">
+        <v>45799</v>
+      </c>
+      <c r="J17" t="s">
+        <v>126</v>
+      </c>
+      <c r="K17" t="s">
+        <v>125</v>
+      </c>
+      <c r="L17" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>127</v>
+      </c>
+      <c r="R17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="2">
+        <v>45590</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" t="s">
+        <v>39</v>
+      </c>
+      <c r="H18" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="2">
+        <v>45799</v>
+      </c>
+      <c r="J18" t="s">
+        <v>126</v>
+      </c>
+      <c r="K18" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>128</v>
+      </c>
+      <c r="R18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="2">
+        <v>45590</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" t="s">
+        <v>39</v>
+      </c>
+      <c r="H19" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="2">
+        <v>45799</v>
+      </c>
+      <c r="J19" t="s">
+        <v>126</v>
+      </c>
+      <c r="K19" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>129</v>
+      </c>
+      <c r="R19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="2">
+        <v>45124</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" t="s">
+        <v>133</v>
+      </c>
+      <c r="H20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="2">
+        <v>45799</v>
+      </c>
+      <c r="J20" t="s">
+        <v>126</v>
+      </c>
+      <c r="K20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" s="2">
+        <v>45119</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" t="s">
+        <v>135</v>
+      </c>
+      <c r="H21" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="2">
+        <v>45799</v>
+      </c>
+      <c r="J21" t="s">
+        <v>126</v>
+      </c>
+      <c r="K21" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" t="s">
+        <v>70</v>
+      </c>
+      <c r="H22" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="2">
+        <v>45799</v>
+      </c>
+      <c r="J22" t="s">
+        <v>126</v>
+      </c>
+      <c r="K22" t="s">
+        <v>125</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="2">
+        <v>45799</v>
+      </c>
+      <c r="J23" t="s">
+        <v>126</v>
+      </c>
+      <c r="K23" t="s">
+        <v>125</v>
+      </c>
+      <c r="R23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="2">
+        <v>45799</v>
+      </c>
+      <c r="J24" t="s">
+        <v>126</v>
+      </c>
+      <c r="K24" t="s">
+        <v>125</v>
+      </c>
+      <c r="R24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E25" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="2">
+        <v>45799</v>
+      </c>
+      <c r="J25" t="s">
+        <v>126</v>
+      </c>
+      <c r="K25" t="s">
+        <v>125</v>
+      </c>
+      <c r="R25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H26" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="2">
+        <v>45799</v>
+      </c>
+      <c r="J26" t="s">
+        <v>126</v>
+      </c>
+      <c r="K26" t="s">
+        <v>125</v>
+      </c>
+      <c r="R26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>70</v>
+      </c>
+      <c r="H27" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="2">
+        <v>45799</v>
+      </c>
+      <c r="J27" t="s">
+        <v>126</v>
+      </c>
+      <c r="K27" t="s">
+        <v>125</v>
+      </c>
+      <c r="R27" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E28" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="2">
+        <v>45799</v>
+      </c>
+      <c r="J28" t="s">
+        <v>126</v>
+      </c>
+      <c r="K28" t="s">
+        <v>125</v>
+      </c>
+      <c r="R28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" t="s">
+        <v>119</v>
+      </c>
+      <c r="D29" s="2">
+        <v>45597</v>
+      </c>
+      <c r="E29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="2">
+        <v>45799</v>
+      </c>
+      <c r="J29" t="s">
+        <v>126</v>
+      </c>
+      <c r="K29" t="s">
+        <v>125</v>
+      </c>
+      <c r="R29" t="s">
+        <v>124</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>